<commit_message>
Corrected invalid data files
</commit_message>
<xml_diff>
--- a/data/2017-08-18_seq11_Huh7_eGFP_CHX.xlsx
+++ b/data/2017-08-18_seq11_Huh7_eGFP_CHX.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="2">
   <si>
     <t xml:space="preserve">t</t>
   </si>
@@ -123,7 +123,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BX121"/>
+  <dimension ref="A1:BL121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -134,7 +134,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -325,42 +325,6 @@
         <v>1</v>
       </c>
       <c r="BL1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="BM1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="BN1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="BO1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="BP1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="BQ1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="BR1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="BS1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="BT1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="BU1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="BV1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="BW1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="BX1" s="0" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>